<commit_message>
1. updata 20230321 2.  修正了定投权重公式
</commit_message>
<xml_diff>
--- a/500低波医药消费策略指数.xlsx
+++ b/500低波医药消费策略指数.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B6319F-8E6C-4F5B-B8D0-4483E102DDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05279FA2-191F-404D-84EC-3C3B91E5B55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="基本参数" sheetId="1" r:id="rId1"/>
-    <sheet name="富国500低波医药消费策略指数 20221030" sheetId="2" r:id="rId2"/>
+    <sheet name="富国500低波医药消费策略指数 20230320" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" concurrentManualCount="12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1418,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F952F159-CCE4-47E5-A079-7D80BB1CE1C7}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2160,285 +2153,301 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="13">
+      <c r="A21" s="16">
         <v>2022</v>
       </c>
-      <c r="B21" s="14">
-        <v>3541</v>
-      </c>
-      <c r="C21" s="14">
-        <v>5781</v>
-      </c>
-      <c r="D21" s="14">
-        <v>14206</v>
-      </c>
-      <c r="E21" s="14">
-        <v>13218</v>
-      </c>
-      <c r="F21" s="14">
-        <v>17907</v>
-      </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15">
+      <c r="B21" s="16">
+        <v>3871</v>
+      </c>
+      <c r="C21" s="16">
+        <v>5864</v>
+      </c>
+      <c r="D21" s="20">
+        <v>14690</v>
+      </c>
+      <c r="E21" s="16">
+        <v>13504</v>
+      </c>
+      <c r="F21" s="16">
+        <v>21573</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17">
         <f t="shared" ref="H21" si="11">(B21-B20)/B20</f>
-        <v>-0.28319838056680163</v>
-      </c>
-      <c r="I21" s="15">
+        <v>-0.21639676113360323</v>
+      </c>
+      <c r="I21" s="17">
         <f t="shared" ref="I21" si="12">(C21-C20)/C20</f>
-        <v>-0.21443130860171219</v>
-      </c>
-      <c r="J21" s="15">
+        <v>-0.20315260225574128</v>
+      </c>
+      <c r="J21" s="17">
         <f t="shared" ref="J21" si="13">(D21-D20)/D20</f>
-        <v>-0.17751273737841594</v>
-      </c>
-      <c r="K21" s="15">
+        <v>-0.14949050486336266</v>
+      </c>
+      <c r="K21" s="17">
         <f t="shared" ref="K21" si="14">(E21-E20)/E20</f>
-        <v>-0.21363555238265214</v>
-      </c>
-      <c r="L21" s="15">
+        <v>-0.1966208578737581</v>
+      </c>
+      <c r="L21" s="17">
         <f t="shared" ref="L21" si="15">(F21-F20)/F20</f>
-        <v>-0.28985564720812185</v>
+        <v>-0.14447176395939088</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="A22" s="13">
+        <v>2023</v>
+      </c>
+      <c r="B22" s="14">
+        <v>3939</v>
+      </c>
+      <c r="C22" s="14">
+        <v>6160</v>
+      </c>
+      <c r="D22" s="14">
+        <v>16070</v>
+      </c>
+      <c r="E22" s="14">
+        <v>13391</v>
+      </c>
+      <c r="F22" s="14">
+        <v>21034</v>
+      </c>
       <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
+      <c r="H22" s="15">
+        <f t="shared" ref="H22" si="16">(B22-B21)/B21</f>
+        <v>1.7566520278997674E-2</v>
+      </c>
+      <c r="I22" s="15">
+        <f t="shared" ref="I22" si="17">(C22-C21)/C21</f>
+        <v>5.0477489768076401E-2</v>
+      </c>
+      <c r="J22" s="15">
+        <f t="shared" ref="J22" si="18">(D22-D21)/D21</f>
+        <v>9.3941456773315182E-2</v>
+      </c>
+      <c r="K22" s="15">
+        <f t="shared" ref="K22" si="19">(E22-E21)/E21</f>
+        <v>-8.3678909952606632E-3</v>
+      </c>
+      <c r="L22" s="15">
+        <f t="shared" ref="L22" si="20">(F22-F21)/F21</f>
+        <v>-2.4984934872294071E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="20">
-        <f>B19+B19*H28</f>
-        <v>5590.2093092981868</v>
-      </c>
-      <c r="C23" s="20">
-        <f t="shared" ref="C23:F23" si="16">C19+C19*I28</f>
-        <v>7018.888577090087</v>
-      </c>
-      <c r="D23" s="20">
-        <f t="shared" si="16"/>
-        <v>16648.000252197406</v>
-      </c>
-      <c r="E23" s="20">
-        <f t="shared" si="16"/>
-        <v>20434.235155234262</v>
-      </c>
-      <c r="F23" s="20">
-        <f t="shared" si="16"/>
-        <v>32204.558091518484</v>
-      </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="17">
-        <f>H28</f>
-        <v>7.2770928669772861E-2</v>
-      </c>
-      <c r="I23" s="17">
-        <f t="shared" ref="I23:L23" si="17">I28</f>
-        <v>0.10238551548454322</v>
-      </c>
-      <c r="J23" s="17">
-        <f t="shared" si="17"/>
-        <v>0.15884729585113511</v>
-      </c>
-      <c r="K23" s="17">
-        <f t="shared" si="17"/>
-        <v>0.15421572273126194</v>
-      </c>
-      <c r="L23" s="17">
-        <f t="shared" si="17"/>
-        <v>0.17384939280184009</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
+      <c r="B24" s="20">
+        <f>B19+B19*H29</f>
+        <v>5623.3882887703858</v>
+      </c>
+      <c r="C24" s="20">
+        <f t="shared" ref="C24:F24" si="21">C19+C19*I29</f>
+        <v>7043.6934223487369</v>
+      </c>
+      <c r="D24" s="20">
+        <f t="shared" si="21"/>
+        <v>16762.421002766474</v>
+      </c>
+      <c r="E24" s="20">
+        <f t="shared" si="21"/>
+        <v>20449.002296323662</v>
+      </c>
+      <c r="F24" s="20">
+        <f t="shared" si="21"/>
+        <v>32493.809045885042</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17">
+        <f>H29</f>
+        <v>7.9138032771135292E-2</v>
+      </c>
+      <c r="I24" s="17">
+        <f t="shared" ref="I24:L24" si="22">I29</f>
+        <v>0.10628136050710491</v>
+      </c>
+      <c r="J24" s="17">
+        <f t="shared" si="22"/>
+        <v>0.16681198682768161</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="22"/>
+        <v>0.15504983598755429</v>
+      </c>
+      <c r="L24" s="17">
+        <f t="shared" si="22"/>
+        <v>0.18439252946546536</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="22">
-        <f>B20-B23</f>
-        <v>-650.20930929818678</v>
-      </c>
-      <c r="C24" s="22">
-        <f t="shared" ref="C24:F24" si="18">C20-C23</f>
-        <v>340.11142290991302</v>
-      </c>
-      <c r="D24" s="22">
-        <f t="shared" si="18"/>
-        <v>623.99974780259436</v>
-      </c>
-      <c r="E24" s="22">
-        <f t="shared" si="18"/>
-        <v>-3625.2351552342625</v>
-      </c>
-      <c r="F24" s="22">
-        <f t="shared" si="18"/>
-        <v>-6988.5580915184837</v>
-      </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="15">
-        <f>H21-H23</f>
-        <v>-0.35596930923657449</v>
-      </c>
-      <c r="I24" s="15">
-        <f t="shared" ref="I24:L24" si="19">I21-I23</f>
-        <v>-0.31681682408625544</v>
-      </c>
-      <c r="J24" s="15">
-        <f t="shared" si="19"/>
-        <v>-0.33636003322955105</v>
-      </c>
-      <c r="K24" s="15">
-        <f t="shared" si="19"/>
-        <v>-0.36785127511391408</v>
-      </c>
-      <c r="L24" s="15">
-        <f t="shared" si="19"/>
-        <v>-0.46370504000996193</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
+      <c r="B25" s="22">
+        <f>B20-B24</f>
+        <v>-683.38828877038577</v>
+      </c>
+      <c r="C25" s="22">
+        <f t="shared" ref="C25:F25" si="23">C20-C24</f>
+        <v>315.30657765126307</v>
+      </c>
+      <c r="D25" s="22">
+        <f t="shared" si="23"/>
+        <v>509.57899723352602</v>
+      </c>
+      <c r="E25" s="22">
+        <f t="shared" si="23"/>
+        <v>-3640.0022963236624</v>
+      </c>
+      <c r="F25" s="22">
+        <f t="shared" si="23"/>
+        <v>-7277.809045885042</v>
+      </c>
+      <c r="G25" s="22"/>
+      <c r="H25" s="15">
+        <f>H22-H24</f>
+        <v>-6.1571512492137617E-2</v>
+      </c>
+      <c r="I25" s="15">
+        <f t="shared" ref="I25:L25" si="24">I22-I24</f>
+        <v>-5.5803870739028504E-2</v>
+      </c>
+      <c r="J25" s="15">
+        <f t="shared" si="24"/>
+        <v>-7.2870530054366431E-2</v>
+      </c>
+      <c r="K25" s="15">
+        <f t="shared" si="24"/>
+        <v>-0.16341772698281495</v>
+      </c>
+      <c r="L25" s="15">
+        <f t="shared" si="24"/>
+        <v>-0.20937746433775944</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="17">
-        <f>(B21/1000)</f>
-        <v>3.5409999999999999</v>
-      </c>
-      <c r="I27" s="17">
-        <f t="shared" ref="I27:L27" si="20">(C21/1000)</f>
-        <v>5.7809999999999997</v>
-      </c>
-      <c r="J27" s="17">
-        <f t="shared" si="20"/>
-        <v>14.206</v>
-      </c>
-      <c r="K27" s="17">
-        <f t="shared" si="20"/>
-        <v>13.218</v>
-      </c>
-      <c r="L27" s="17">
-        <f t="shared" si="20"/>
-        <v>17.907</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A28" s="35" t="s">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17">
+        <f>(B22/1000)</f>
+        <v>3.9390000000000001</v>
+      </c>
+      <c r="I28" s="17">
+        <f t="shared" ref="I28:L28" si="25">(C22/1000)</f>
+        <v>6.16</v>
+      </c>
+      <c r="J28" s="17">
+        <f t="shared" si="25"/>
+        <v>16.07</v>
+      </c>
+      <c r="K28" s="17">
+        <f t="shared" si="25"/>
+        <v>13.391</v>
+      </c>
+      <c r="L28" s="17">
+        <f t="shared" si="25"/>
+        <v>21.033999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="23">
-        <f>POWER(H27,(1/18))-1</f>
-        <v>7.2770928669772861E-2</v>
-      </c>
-      <c r="I28" s="23">
-        <f t="shared" ref="I28:L28" si="21">POWER(I27,(1/18))-1</f>
-        <v>0.10238551548454322</v>
-      </c>
-      <c r="J28" s="23">
-        <f t="shared" si="21"/>
-        <v>0.15884729585113511</v>
-      </c>
-      <c r="K28" s="23">
-        <f t="shared" si="21"/>
-        <v>0.15421572273126194</v>
-      </c>
-      <c r="L28" s="23">
-        <f t="shared" si="21"/>
-        <v>0.17384939280184009</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-    </row>
-    <row r="30" spans="1:15" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="35" t="s">
+      <c r="H29" s="23">
+        <f>POWER(H28,(1/18))-1</f>
+        <v>7.9138032771135292E-2</v>
+      </c>
+      <c r="I29" s="23">
+        <f t="shared" ref="I29:L29" si="26">POWER(I28,(1/18))-1</f>
+        <v>0.10628136050710491</v>
+      </c>
+      <c r="J29" s="23">
+        <f t="shared" si="26"/>
+        <v>0.16681198682768161</v>
+      </c>
+      <c r="K29" s="23">
+        <f t="shared" si="26"/>
+        <v>0.15504983598755429</v>
+      </c>
+      <c r="L29" s="23">
+        <f t="shared" si="26"/>
+        <v>0.18439252946546536</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="6" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+    </row>
+    <row r="31" spans="1:15" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="23">
-        <f>(K24+L24)/(J24+K24+L24)</f>
-        <v>0.71199989305418654</v>
-      </c>
-      <c r="K30" s="23">
-        <f>(J24+L24)/(J24+K24+L24)</f>
-        <v>0.68503628223671598</v>
-      </c>
-      <c r="L30" s="23">
-        <f>(J24+K24)/(J24+K24+L24)</f>
-        <v>0.6029638247090976</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="35" t="s">
-        <v>18</v>
-      </c>
       <c r="B31" s="36"/>
-      <c r="C31" s="26"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -2446,66 +2455,75 @@
       <c r="H31" s="25"/>
       <c r="I31" s="25"/>
       <c r="J31" s="23">
-        <f>J30/($J$30+$K$30+$L$30)</f>
-        <v>0.35599994652709327</v>
+        <f>(K22+L22)/(J22+K22+L22)</f>
+        <v>-0.55047993937066708</v>
       </c>
       <c r="K31" s="23">
-        <f>K30/($J$30+$K$30+$L$30)</f>
-        <v>0.34251814111835799</v>
+        <f>(J22+L22)/(J22+K22+L22)</f>
+        <v>1.138109920461416</v>
       </c>
       <c r="L31" s="23">
-        <f>L30/($J$30+$K$30+$L$30)</f>
-        <v>0.3014819123545488</v>
-      </c>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
+        <f>(J22+K22)/(J22+K22+L22)</f>
+        <v>1.4123700189092512</v>
+      </c>
     </row>
     <row r="32" spans="1:15" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="23">
+        <f>J31/($J$31+$K$31+$L$31)</f>
+        <v>-0.27523996968533354</v>
+      </c>
+      <c r="K32" s="23">
+        <f>K31/($J$31+$K$31+$L$31)</f>
+        <v>0.56905496023070801</v>
+      </c>
+      <c r="L32" s="23">
+        <f>L31/($J$31+$K$31+$L$31)</f>
+        <v>0.70618500945462559</v>
+      </c>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+    </row>
+    <row r="33" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="14">
-        <v>900</v>
-      </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="29">
-        <f>$C$32*J31</f>
-        <v>320.39995187438393</v>
-      </c>
-      <c r="K32" s="29">
-        <f t="shared" ref="K32:L32" si="22">$C$32*K31</f>
-        <v>308.2663270065222</v>
-      </c>
-      <c r="L32" s="29">
-        <f t="shared" si="22"/>
-        <v>271.33372111909392</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="14">
+        <v>5000</v>
+      </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-    </row>
-    <row r="34" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="J33" s="29">
+        <f>$C$33*J32</f>
+        <v>-1376.1998484266678</v>
+      </c>
+      <c r="K33" s="29">
+        <f t="shared" ref="K33:L33" si="27">$C$33*K32</f>
+        <v>2845.27480115354</v>
+      </c>
+      <c r="L33" s="29">
+        <f t="shared" si="27"/>
+        <v>3530.9250472731278</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
@@ -2514,26 +2532,42 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
       <c r="I34" s="21"/>
-      <c r="J34" s="23">
-        <f>J31*0.9</f>
-        <v>0.32039995187438397</v>
-      </c>
-      <c r="K34" s="23">
-        <f t="shared" ref="K34:L34" si="23">K31*0.9</f>
-        <v>0.30826632700652218</v>
-      </c>
-      <c r="L34" s="23">
-        <f t="shared" si="23"/>
-        <v>0.27133372111909393</v>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+    </row>
+    <row r="35" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="23">
+        <f>J32*0.9</f>
+        <v>-0.24771597271680018</v>
+      </c>
+      <c r="K35" s="23">
+        <f t="shared" ref="K35:L35" si="28">K32*0.9</f>
+        <v>0.51214946420763718</v>
+      </c>
+      <c r="L35" s="23">
+        <f t="shared" si="28"/>
+        <v>0.63556650850916308</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="H1:L1"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>